<commit_message>
Some work on tree replacements
</commit_message>
<xml_diff>
--- a/Trees/STO/Replacement tracking/Tree replacements.xlsx
+++ b/Trees/STO/Replacement tracking/Tree replacements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kent/Dev/Noho/Trees/STO/Replacement tracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB854490-BEDE-CA46-98C0-5C5AA0C4C150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F684CDF-CC53-EF40-B4CD-EEDE78E21E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="3520" windowWidth="27920" windowHeight="13920" xr2:uid="{B7658DB7-84F7-914E-8320-8DBFC49D6E54}"/>
+    <workbookView xWindow="10120" yWindow="2780" windowWidth="34360" windowHeight="16580" xr2:uid="{B7658DB7-84F7-914E-8320-8DBFC49D6E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="140">
   <si>
     <t>Permit</t>
   </si>
@@ -203,15 +203,9 @@
     <t>Winterberry</t>
   </si>
   <si>
-    <t>6+</t>
-  </si>
-  <si>
     <t>Planning Board Spec. Permit/Site</t>
   </si>
   <si>
-    <t>Hinckley St</t>
-  </si>
-  <si>
     <t>Wright Builders/Sweet Mea</t>
   </si>
   <si>
@@ -323,9 +317,6 @@
     <t>City-Department of Public Works</t>
   </si>
   <si>
-    <t>Main St, Florence</t>
-  </si>
-  <si>
     <t>Bridge St/Pomeroy Terrace</t>
   </si>
   <si>
@@ -399,6 +390,72 @@
   </si>
   <si>
     <t>19 @-22"</t>
+  </si>
+  <si>
+    <t>Map-Lot</t>
+  </si>
+  <si>
+    <t>29 -111-001</t>
+  </si>
+  <si>
+    <t>18C-048-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30D-019-001  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">32C-198-001 </t>
+  </si>
+  <si>
+    <t>Payment-In-Lieu Amount</t>
+  </si>
+  <si>
+    <t>23A-031-001</t>
+  </si>
+  <si>
+    <t>34 -034-001</t>
+  </si>
+  <si>
+    <t>25A-132-001</t>
+  </si>
+  <si>
+    <t>23B-047-001</t>
+  </si>
+  <si>
+    <t>35 -156-001</t>
+  </si>
+  <si>
+    <t>31B-216-001</t>
+  </si>
+  <si>
+    <t>17C-197-001</t>
+  </si>
+  <si>
+    <t>53 Main St, Florence</t>
+  </si>
+  <si>
+    <t>31C-17</t>
+  </si>
+  <si>
+    <t>31B-004</t>
+  </si>
+  <si>
+    <t>32A-185</t>
+  </si>
+  <si>
+    <t>121 Hinckley St</t>
+  </si>
+  <si>
+    <t>23D-149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32C-058-001 </t>
+  </si>
+  <si>
+    <t>38A-108-001</t>
+  </si>
+  <si>
+    <t>21 Olander Dr</t>
   </si>
 </sst>
 </file>
@@ -443,13 +500,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,63 +844,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0523DA52-5DB1-9B4F-A159-084559E38D0B}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -851,22 +920,25 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>79</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -877,25 +949,28 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>162</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>81</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -906,28 +981,31 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>76</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -938,25 +1016,28 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>56</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>8</v>
       </c>
-      <c r="H5">
-        <v>28</v>
-      </c>
       <c r="I5">
+        <v>19.5</v>
+      </c>
+      <c r="J5">
         <v>9.5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -967,28 +1048,31 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="F6">
-        <v>103</v>
-      </c>
       <c r="G6">
+        <v>146</v>
+      </c>
+      <c r="H6">
         <v>13</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>26</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>47</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -999,28 +1083,31 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>348</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>55</v>
-      </c>
-      <c r="H7">
-        <v>64</v>
       </c>
       <c r="I7">
         <v>64</v>
       </c>
-      <c r="L7" t="s">
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="N7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1031,28 +1118,31 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>50</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>25</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1063,25 +1153,28 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>64</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>18</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>50</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1092,25 +1185,28 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>108</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>25</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>60</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1121,28 +1217,31 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>57</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>15</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>29</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1153,25 +1252,28 @@
         <v>42</v>
       </c>
       <c r="D12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>40</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>14</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>32</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1179,28 +1281,37 @@
         <v>42491</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="D13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>3</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>62</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>5</v>
       </c>
-      <c r="I13" s="4">
-        <v>4320</v>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>47</v>
       </c>
       <c r="K13" s="4">
         <v>4320</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="4">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1211,22 +1322,28 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14">
         <v>14</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>280</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>46</v>
       </c>
-      <c r="J14">
+      <c r="I14">
+        <v>126</v>
+      </c>
+      <c r="L14">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1237,25 +1354,31 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>13</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>364</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>21</v>
       </c>
-      <c r="J15">
+      <c r="I15">
+        <v>65</v>
+      </c>
+      <c r="L15">
         <v>21</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1265,26 +1388,29 @@
       <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16">
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16">
         <v>1</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>24</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>6</v>
       </c>
-      <c r="J16">
+      <c r="I16">
+        <v>12</v>
+      </c>
+      <c r="L16">
         <v>6</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1292,95 +1418,110 @@
         <v>42552</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
         <v>54</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>1</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>24</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>15</v>
+      </c>
+      <c r="L17">
+        <v>6</v>
+      </c>
+      <c r="M17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>55</v>
-      </c>
-      <c r="J17">
-        <v>6</v>
-      </c>
-      <c r="K17">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>56</v>
       </c>
       <c r="B18" s="3">
         <v>42614</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18">
+        <v>136</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18">
         <v>2</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>72</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>14</v>
       </c>
-      <c r="I18" s="4">
-        <v>1800</v>
-      </c>
-      <c r="J18">
-        <v>14</v>
+      <c r="I18">
+        <v>18</v>
       </c>
       <c r="K18" s="4">
         <v>1800</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18">
+        <v>14</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1800</v>
+      </c>
+      <c r="N18" s="1">
         <v>42997</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="3">
         <v>44317</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19">
+        <v>136</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>56</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="4">
+      <c r="K19" s="4">
         <v>2800</v>
       </c>
-      <c r="K19" s="4">
+      <c r="M19" s="4">
         <v>2100</v>
       </c>
-      <c r="L19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1388,25 +1529,31 @@
         <v>42705</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20">
+        <v>137</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20">
         <v>3</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>68</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>8</v>
       </c>
-      <c r="J20">
+      <c r="I20">
+        <v>34</v>
+      </c>
+      <c r="L20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1414,74 +1561,80 @@
         <v>42767</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21">
+        <v>138</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21">
         <v>11</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>292</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>65</v>
       </c>
-      <c r="J21">
+      <c r="I21">
+        <v>165</v>
+      </c>
+      <c r="L21">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" s="3">
         <v>42887</v>
       </c>
       <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>234</v>
+      </c>
+      <c r="H22">
+        <v>23</v>
+      </c>
+      <c r="K22" s="4">
+        <v>5500</v>
+      </c>
+      <c r="N22" t="s">
         <v>65</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="E22">
-        <v>12</v>
-      </c>
-      <c r="F22">
-        <v>234</v>
-      </c>
-      <c r="G22">
-        <v>23</v>
-      </c>
-      <c r="I22" s="4">
-        <v>5500</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="K23" s="5">
+        <v>2000</v>
+      </c>
+      <c r="M23" s="4">
+        <v>2000</v>
+      </c>
+      <c r="N23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <v>40</v>
-      </c>
-      <c r="I23" s="5">
-        <v>2000</v>
-      </c>
-      <c r="K23" s="4">
-        <v>2000</v>
-      </c>
-      <c r="L23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1489,82 +1642,82 @@
         <v>42887</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24">
+        <v>95</v>
+      </c>
+      <c r="E24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24">
         <v>1</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>30</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>7</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K24" s="5"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" s="3">
         <v>42948</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25">
         <v>4</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>116</v>
-      </c>
-      <c r="I25">
-        <v>600</v>
-      </c>
-      <c r="J25" t="s">
-        <v>100</v>
       </c>
       <c r="K25">
         <v>600</v>
       </c>
       <c r="L25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="M25">
+        <v>600</v>
+      </c>
+      <c r="N25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="3">
         <v>42948</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26">
         <v>2</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>55</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>28</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1574,130 +1727,130 @@
       <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27">
         <v>1</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>34</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>5</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>5</v>
       </c>
-      <c r="L27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="3">
         <v>42614</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28">
+        <v>76</v>
+      </c>
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28">
         <v>16</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>413</v>
       </c>
-      <c r="I28" s="4">
+      <c r="K28" s="4">
         <v>8325</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="3">
         <v>42614</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="E29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="3">
         <v>43009</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30">
         <v>30</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>704</v>
       </c>
-      <c r="G30">
-        <v>16</v>
-      </c>
-      <c r="I30" s="4">
-        <v>30900</v>
-      </c>
-      <c r="J30">
+      <c r="H30">
         <v>16</v>
       </c>
       <c r="K30" s="4">
         <v>30900</v>
       </c>
-      <c r="L30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>16</v>
+      </c>
+      <c r="M30" s="4">
+        <v>30900</v>
+      </c>
+      <c r="N30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B31" s="3">
         <v>43435</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31">
         <v>247</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>6916</v>
-      </c>
-      <c r="I31" s="4">
-        <v>318800</v>
-      </c>
-      <c r="J31">
-        <v>90</v>
       </c>
       <c r="K31" s="4">
         <v>318800</v>
       </c>
-      <c r="L31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>90</v>
+      </c>
+      <c r="M31" s="4">
+        <v>318800</v>
+      </c>
+      <c r="N31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1705,147 +1858,147 @@
         <v>43405</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32">
+        <v>103</v>
+      </c>
+      <c r="E32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32">
         <v>80</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>1843</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>461</v>
-      </c>
-      <c r="I32" s="4">
-        <v>86000</v>
-      </c>
-      <c r="J32">
-        <v>110</v>
       </c>
       <c r="K32" s="4">
         <v>86000</v>
       </c>
-      <c r="L32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>110</v>
+      </c>
+      <c r="M32" s="4">
+        <v>86000</v>
+      </c>
+      <c r="N32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B33" s="3">
         <v>43374</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33">
+        <v>106</v>
+      </c>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33">
         <v>20</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>547</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>110</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>110</v>
       </c>
-      <c r="L33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B34" s="3">
         <v>43344</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34">
+        <v>108</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34">
         <v>1</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>24</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>6</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>6</v>
       </c>
-      <c r="L34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" s="3">
         <v>43101</v>
       </c>
       <c r="C35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35">
+        <v>15</v>
+      </c>
+      <c r="G35">
+        <v>389</v>
+      </c>
+      <c r="H35">
+        <v>98</v>
+      </c>
+      <c r="L35">
         <v>86</v>
       </c>
-      <c r="D35" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35">
-        <v>15</v>
-      </c>
-      <c r="F35">
-        <v>389</v>
-      </c>
-      <c r="G35">
-        <v>98</v>
-      </c>
-      <c r="J35">
-        <v>86</v>
-      </c>
-      <c r="L35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B36" s="3">
         <v>43617</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" t="s">
-        <v>88</v>
-      </c>
-      <c r="E36">
+        <v>111</v>
+      </c>
+      <c r="E36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36">
         <v>9</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>268</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>70</v>
       </c>
-      <c r="L36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1853,120 +2006,120 @@
         <v>43525</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" t="s">
-        <v>89</v>
-      </c>
-      <c r="E37">
+        <v>113</v>
+      </c>
+      <c r="E37" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37">
         <v>2</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>42</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>7</v>
-      </c>
-      <c r="I37">
-        <v>750</v>
-      </c>
-      <c r="J37">
-        <v>5</v>
       </c>
       <c r="K37">
         <v>750</v>
       </c>
-      <c r="L37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>5</v>
+      </c>
+      <c r="M37">
+        <v>750</v>
+      </c>
+      <c r="N37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" s="3">
         <v>44256</v>
       </c>
       <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>108</v>
+      </c>
+      <c r="H38" t="s">
         <v>117</v>
-      </c>
-      <c r="D38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
-      </c>
-      <c r="F38">
-        <v>108</v>
-      </c>
-      <c r="G38" t="s">
-        <v>120</v>
-      </c>
-      <c r="I38" s="4">
-        <v>3200</v>
-      </c>
-      <c r="J38">
-        <v>22</v>
       </c>
       <c r="K38" s="4">
         <v>3200</v>
       </c>
-      <c r="L38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>22</v>
+      </c>
+      <c r="M38" s="4">
+        <v>3200</v>
+      </c>
+      <c r="N38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39">
+        <v>90</v>
+      </c>
+      <c r="E39" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39">
         <v>2</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>68</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>5</v>
-      </c>
-      <c r="I39" s="4">
-        <v>3000</v>
-      </c>
-      <c r="J39">
-        <v>2</v>
       </c>
       <c r="K39" s="4">
         <v>3000</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E40">
-        <f>SUM(E13:E39)</f>
-        <v>499</v>
-      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39" s="4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F40">
         <f>SUM(F13:F39)</f>
-        <v>13073</v>
+        <v>499</v>
       </c>
       <c r="G40">
         <f>SUM(G13:G39)</f>
-        <v>1001</v>
-      </c>
-      <c r="I40">
-        <f>SUM(I13:I39)</f>
-        <v>467995</v>
-      </c>
-      <c r="J40">
-        <f>SUM(J13:J39)</f>
-        <v>648</v>
+        <v>13073</v>
+      </c>
+      <c r="H40">
+        <f>SUM(H13:H39)</f>
+        <v>1007</v>
       </c>
       <c r="K40">
         <f>SUM(K13:K39)</f>
+        <v>467995</v>
+      </c>
+      <c r="L40">
+        <f>SUM(L13:L39)</f>
+        <v>648</v>
+      </c>
+      <c r="M40">
+        <f>SUM(M13:M39)</f>
         <v>453720</v>
       </c>
     </row>

</xml_diff>